<commit_message>
add nota unidade 3 - introdução
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,15 +684,20 @@
       <c r="D3" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="1">
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="1">
         <v>10</v>
       </c>
-      <c r="K3">
-        <f>(F3+G3+H3+I3)/4 + J3</f>
-        <v>4.5</v>
+      <c r="H3" s="1">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1">
+        <f>F3+G3+H3+I3+J3</f>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -709,13 +714,13 @@
         <v>27</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5">
-        <f t="shared" ref="K4:K15" si="0">(F4+G4+H4+I4)/4 + J4</f>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="1">
+        <f t="shared" ref="K4:K15" si="0">F4+G4+H4+I4+J4</f>
         <v>0</v>
       </c>
       <c r="L4" s="5"/>
@@ -733,7 +738,12 @@
       <c r="D5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K5">
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -752,12 +762,12 @@
         <v>28</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
-      <c r="K6" s="5">
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="4"/>
+      <c r="K6" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -776,7 +786,12 @@
       <c r="D7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K7">
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -795,12 +810,12 @@
         <v>29</v>
       </c>
       <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="5"/>
-      <c r="J8" s="5"/>
-      <c r="K8" s="5">
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -819,7 +834,12 @@
       <c r="D9" s="2">
         <v>44177</v>
       </c>
-      <c r="K9">
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -838,12 +858,12 @@
         <v>44177</v>
       </c>
       <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="5"/>
-      <c r="K10" s="5">
+      <c r="F10" s="4"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -862,7 +882,12 @@
       <c r="D11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K11">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -881,12 +906,12 @@
         <v>30</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="5"/>
-      <c r="J12" s="5"/>
-      <c r="K12" s="5">
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -905,7 +930,12 @@
       <c r="D13" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="K13">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -924,12 +954,12 @@
         <v>31</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="5"/>
-      <c r="J14" s="5"/>
-      <c r="K14" s="5">
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -948,7 +978,12 @@
       <c r="D15" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="K15">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -959,7 +994,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>0.375</v>
+        <v>2.1666666666666665</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add terceira nota - introdução
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -618,8 +618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -693,11 +693,13 @@
       <c r="H3" s="1">
         <v>8</v>
       </c>
-      <c r="I3" s="1"/>
+      <c r="I3" s="1">
+        <v>6</v>
+      </c>
       <c r="J3" s="1"/>
       <c r="K3" s="1">
         <f>F3+G3+H3+I3+J3</f>
-        <v>26</v>
+        <v>32</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -994,7 +996,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>2.1666666666666665</v>
+        <v>2.6666666666666665</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
atualizando nota primeira disciplina, rumo ao TCC
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
   <si>
     <t>Disciplina</t>
   </si>
@@ -208,6 +208,12 @@
   </si>
   <si>
     <t>Produção</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AP </t>
   </si>
 </sst>
 </file>
@@ -279,7 +285,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -314,6 +320,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -618,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -699,9 +708,12 @@
       <c r="J3" s="1">
         <v>54</v>
       </c>
-      <c r="K3" s="1">
+      <c r="K3" s="14">
         <f>F3+G3+H3+I3+J3</f>
         <v>86</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -727,7 +739,7 @@
         <f t="shared" ref="K4:K15" si="0">F4+G4+H4+I4+J4</f>
         <v>0</v>
       </c>
-      <c r="L4" s="5"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -751,6 +763,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L5" s="1"/>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
@@ -775,7 +788,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L6" s="5"/>
+      <c r="L6" s="1"/>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
@@ -799,6 +812,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
@@ -823,7 +837,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L8" s="5"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
@@ -847,6 +861,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
@@ -871,7 +886,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L10" s="5"/>
+      <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
@@ -895,6 +910,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L11" s="1"/>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -919,7 +935,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L12" s="5"/>
+      <c r="L12" s="4"/>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
@@ -943,6 +959,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="L13" s="1"/>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
@@ -967,7 +984,7 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L14" s="5"/>
+      <c r="L14" s="4"/>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
@@ -1001,10 +1018,10 @@
         <v>7.166666666666667</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>42</v>
@@ -1015,8 +1032,11 @@
       <c r="D18" s="13" t="s">
         <v>44</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="H18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
         <v>43</v>
@@ -1028,7 +1048,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>59</v>
       </c>
@@ -1045,7 +1065,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>58</v>
       </c>
@@ -1062,7 +1082,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>58</v>
       </c>
@@ -1079,7 +1099,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
         <v>51</v>
@@ -1091,7 +1111,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>59</v>
       </c>
@@ -1108,7 +1128,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
         <v>55</v>
@@ -1120,7 +1140,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
         <v>56</v>
@@ -1132,16 +1152,16 @@
         <v>44</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
prova unidade 1 gestão de projetos
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -627,8 +627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,14 +779,16 @@
         <v>28</v>
       </c>
       <c r="E6" s="5"/>
-      <c r="F6" s="4"/>
+      <c r="F6" s="4">
+        <v>8</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
       <c r="K6" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="L6" s="1"/>
     </row>
@@ -1015,7 +1017,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>7.166666666666667</v>
+        <v>7.833333333333333</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add teste unidade 2 - gestão de processos
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -628,7 +628,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -757,13 +757,15 @@
       <c r="F5" s="1">
         <v>10</v>
       </c>
-      <c r="G5" s="1"/>
+      <c r="G5" s="1">
+        <v>10</v>
+      </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L5" s="1"/>
     </row>
@@ -1019,7 +1021,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>8.6666666666666661</v>
+        <v>9.5</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add nota prova unidade 3 gestão de processos
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -628,7 +628,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,12 +760,14 @@
       <c r="G5" s="1">
         <v>10</v>
       </c>
-      <c r="H5" s="1"/>
+      <c r="H5" s="1">
+        <v>10</v>
+      </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="L5" s="1"/>
     </row>
@@ -1021,7 +1023,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>9.5</v>
+        <v>10.333333333333334</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
quarta e ultima teste gestão de processos
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -628,7 +628,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,11 +763,13 @@
       <c r="H5" s="1">
         <v>10</v>
       </c>
-      <c r="I5" s="1"/>
+      <c r="I5" s="1">
+        <v>10</v>
+      </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="L5" s="1"/>
     </row>
@@ -1023,7 +1025,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>10.333333333333334</v>
+        <v>11.166666666666666</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
teste unidade 3 - gestão de projetos
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="65">
   <si>
     <t>Disciplina</t>
   </si>
@@ -249,7 +249,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -268,8 +268,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -277,12 +283,49 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -318,6 +361,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -622,10 +677,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L30"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,12 +693,12 @@
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="10"/>
       <c r="B2" s="11" t="s">
         <v>0</v>
@@ -677,7 +732,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -712,8 +767,11 @@
       <c r="L3" s="1" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" s="15" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -732,13 +790,14 @@
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
       <c r="J4" s="4"/>
-      <c r="K4" s="1">
+      <c r="K4" s="4">
         <f t="shared" ref="K4:K15" si="0">F4+G4+H4+I4+J4</f>
         <v>0</v>
       </c>
       <c r="L4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" s="16"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
         <v>3</v>
       </c>
@@ -769,8 +828,11 @@
         <v>40</v>
       </c>
       <c r="L5" s="1"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -790,16 +852,21 @@
       <c r="G6" s="4">
         <v>10</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="4">
+        <v>8</v>
+      </c>
       <c r="I6" s="4"/>
       <c r="J6" s="4"/>
-      <c r="K6" s="1">
+      <c r="K6" s="4">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="L6" s="1"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="L6" s="4"/>
+      <c r="M6" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="8">
         <v>5</v>
       </c>
@@ -822,8 +889,11 @@
         <v>0</v>
       </c>
       <c r="L7" s="1"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" s="17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -842,13 +912,14 @@
       <c r="H8" s="4"/>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
-      <c r="K8" s="1">
+      <c r="K8" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" s="16"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>7</v>
       </c>
@@ -871,8 +942,9 @@
         <v>0</v>
       </c>
       <c r="L9" s="1"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" s="16"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -891,13 +963,14 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="1">
+      <c r="K10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="8">
         <v>9</v>
       </c>
@@ -920,8 +993,9 @@
         <v>0</v>
       </c>
       <c r="L11" s="1"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" s="16"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>10</v>
       </c>
@@ -940,13 +1014,14 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="1">
+      <c r="K12" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L12" s="4"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" s="16"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
         <v>11</v>
       </c>
@@ -969,8 +1044,9 @@
         <v>0</v>
       </c>
       <c r="L13" s="1"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" s="16"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
@@ -989,13 +1065,14 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="1">
+      <c r="K14" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L14" s="4"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" s="18"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>13</v>
       </c>
@@ -1018,13 +1095,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J16" s="11" t="s">
         <v>40</v>
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>12</v>
+        <v>12.666666666666666</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prova unidade 4 gestão de projetos
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -680,7 +680,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,11 +855,13 @@
       <c r="H6" s="4">
         <v>8</v>
       </c>
-      <c r="I6" s="4"/>
+      <c r="I6" s="4">
+        <v>10</v>
+      </c>
       <c r="J6" s="4"/>
       <c r="K6" s="4">
         <f t="shared" si="0"/>
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="17" t="s">
@@ -1101,7 +1103,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>12.666666666666666</v>
+        <v>13.5</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
nota prova gestão de projetos 54/60
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -680,7 +680,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I19" sqref="I19"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -858,10 +858,12 @@
       <c r="I6" s="4">
         <v>10</v>
       </c>
-      <c r="J6" s="4"/>
+      <c r="J6" s="4">
+        <v>54</v>
+      </c>
       <c r="K6" s="4">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="L6" s="4"/>
       <c r="M6" s="17" t="s">
@@ -1103,7 +1105,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>13.5</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prova gestão de processos 60/60
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -680,7 +680,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,10 +822,12 @@
       <c r="I5" s="1">
         <v>10</v>
       </c>
-      <c r="J5" s="1"/>
+      <c r="J5" s="1">
+        <v>60</v>
+      </c>
       <c r="K5" s="1">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>100</v>
       </c>
       <c r="L5" s="1"/>
       <c r="M5" s="17" t="s">
@@ -1105,7 +1107,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
teste 01 - modelagem parametrica
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
   <si>
     <t>Disciplina</t>
   </si>
@@ -102,9 +102,6 @@
     <t>27/06/2020</t>
   </si>
   <si>
-    <t>24/10/2020</t>
-  </si>
-  <si>
     <t>24/04/2021</t>
   </si>
   <si>
@@ -214,6 +211,12 @@
   </si>
   <si>
     <t>AP</t>
+  </si>
+  <si>
+    <t>29/10/2020</t>
+  </si>
+  <si>
+    <t>29/08/2020</t>
   </si>
 </sst>
 </file>
@@ -379,10 +382,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -688,8 +691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,7 +707,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -720,25 +723,25 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>38</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -774,10 +777,10 @@
         <v>86</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M3" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -839,10 +842,10 @@
         <v>100</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -856,7 +859,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="4">
@@ -879,10 +882,10 @@
         <v>90</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M6" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -896,20 +899,22 @@
         <v>43898</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="1"/>
+        <v>66</v>
+      </c>
+      <c r="F7" s="1">
+        <v>10</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="17" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -923,7 +928,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>28</v>
+        <v>65</v>
       </c>
       <c r="E8" s="5"/>
       <c r="F8" s="4"/>
@@ -1000,7 +1005,7 @@
         <v>44410</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1025,7 +1030,7 @@
         <v>21</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
@@ -1051,7 +1056,7 @@
         <v>22</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1076,7 +1081,7 @@
         <v>23</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
@@ -1102,7 +1107,7 @@
         <v>24</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1116,11 +1121,11 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J16" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>23</v>
+        <v>23.833333333333332</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1129,189 +1134,189 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E18" s="19"/>
-      <c r="F18" s="19"/>
-      <c r="G18" s="19"/>
-      <c r="H18" s="19"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="19"/>
-      <c r="K18" s="19"/>
+        <v>42</v>
+      </c>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="20"/>
+      <c r="H18" s="20"/>
+      <c r="I18" s="20"/>
+      <c r="J18" s="20"/>
+      <c r="K18" s="20"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E19" s="19"/>
-      <c r="F19" s="19"/>
-      <c r="G19" s="19"/>
-      <c r="H19" s="19"/>
-      <c r="I19" s="19"/>
-      <c r="J19" s="19"/>
-      <c r="K19" s="19"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="20"/>
+      <c r="H19" s="20"/>
+      <c r="I19" s="20"/>
+      <c r="J19" s="20"/>
+      <c r="K19" s="20"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C20" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" t="s">
-        <v>45</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E20" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="F20" s="20"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="20"/>
-      <c r="J20" s="20"/>
-      <c r="K20" s="20"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B21" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E21" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="F21" s="20"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="20"/>
-      <c r="I21" s="20"/>
-      <c r="J21" s="20"/>
-      <c r="K21" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="F21" s="19"/>
+      <c r="G21" s="19"/>
+      <c r="H21" s="19"/>
+      <c r="I21" s="19"/>
+      <c r="J21" s="19"/>
+      <c r="K21" s="19"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
         <v>48</v>
       </c>
-      <c r="C22" t="s">
-        <v>49</v>
-      </c>
       <c r="D22" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E22" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="F22" s="20"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="20"/>
-      <c r="K22" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="F22" s="19"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="19"/>
+      <c r="I22" s="19"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
+        <v>49</v>
+      </c>
+      <c r="C23" t="s">
         <v>50</v>
       </c>
-      <c r="C23" t="s">
-        <v>51</v>
-      </c>
       <c r="D23" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
-      <c r="J23" s="20"/>
-      <c r="K23" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="E23" s="19"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
+      <c r="J23" s="19"/>
+      <c r="K23" s="19"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" t="s">
         <v>52</v>
       </c>
-      <c r="C24" t="s">
-        <v>53</v>
-      </c>
       <c r="D24" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E24" s="20" t="s">
-        <v>60</v>
-      </c>
-      <c r="F24" s="20"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="20"/>
-      <c r="I24" s="20"/>
-      <c r="J24" s="20"/>
-      <c r="K24" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19"/>
+      <c r="H24" s="19"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="19"/>
+      <c r="K24" s="19"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="20"/>
-      <c r="I25" s="20"/>
-      <c r="J25" s="20"/>
-      <c r="K25" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="E25" s="19"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="19"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="19"/>
+      <c r="K25" s="19"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" t="s">
         <v>55</v>
       </c>
-      <c r="C26" t="s">
-        <v>56</v>
-      </c>
       <c r="D26" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="20"/>
-      <c r="K26" s="20"/>
+        <v>42</v>
+      </c>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
+      <c r="H26" s="19"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="19"/>
+      <c r="K26" s="19"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>

</xml_diff>

<commit_message>
tarefa 2 - modelagem paramétrica
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="66">
   <si>
     <t>Disciplina</t>
   </si>
@@ -66,9 +66,6 @@
     <t>16/03/2020</t>
   </si>
   <si>
-    <t>20/04/2020</t>
-  </si>
-  <si>
     <t>18/05/2020</t>
   </si>
   <si>
@@ -213,10 +210,10 @@
     <t>AP</t>
   </si>
   <si>
-    <t>29/10/2020</t>
-  </si>
-  <si>
     <t>29/08/2020</t>
+  </si>
+  <si>
+    <t>24/10/2020</t>
   </si>
 </sst>
 </file>
@@ -691,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -707,7 +704,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -719,29 +716,29 @@
         <v>1</v>
       </c>
       <c r="D2" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>37</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -755,7 +752,7 @@
         <v>15</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" s="1">
         <v>8</v>
@@ -777,10 +774,10 @@
         <v>86</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="M3" s="15" t="s">
-        <v>56</v>
+        <v>61</v>
+      </c>
+      <c r="M3" s="15">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -790,11 +787,11 @@
       <c r="B4" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>16</v>
+      <c r="C4" s="7">
+        <v>43898</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>27</v>
+        <v>65</v>
       </c>
       <c r="E4" s="5"/>
       <c r="F4" s="4"/>
@@ -807,7 +804,9 @@
         <v>0</v>
       </c>
       <c r="L4" s="4"/>
-      <c r="M4" s="16"/>
+      <c r="M4" s="17">
+        <v>2</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
@@ -817,10 +816,10 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1">
         <v>10</v>
@@ -842,10 +841,10 @@
         <v>100</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="M5" s="17" t="s">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="M5" s="17">
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -856,10 +855,10 @@
         <v>5</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E6" s="5"/>
       <c r="F6" s="4">
@@ -882,10 +881,10 @@
         <v>90</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="M6" s="17" t="s">
-        <v>56</v>
+        <v>63</v>
+      </c>
+      <c r="M6" s="17">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -899,22 +898,24 @@
         <v>43898</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F7" s="1">
         <v>10</v>
       </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1">
+        <v>10</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L7" s="1"/>
-      <c r="M7" s="17" t="s">
-        <v>56</v>
+      <c r="M7" s="17">
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -925,7 +926,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>65</v>
@@ -951,7 +952,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D9" s="2">
         <v>44177</v>
@@ -1005,7 +1006,7 @@
         <v>44410</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
@@ -1027,10 +1028,10 @@
         <v>12</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E12" s="5"/>
       <c r="F12" s="4"/>
@@ -1053,10 +1054,10 @@
         <v>13</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
@@ -1078,10 +1079,10 @@
         <v>14</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E14" s="5"/>
       <c r="F14" s="4"/>
@@ -1104,10 +1105,10 @@
         <v>7</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1121,11 +1122,11 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J16" s="11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>23.833333333333332</v>
+        <v>24.666666666666668</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1134,13 +1135,13 @@
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D18" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="20"/>
       <c r="F18" s="20"/>
@@ -1153,13 +1154,13 @@
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>41</v>
-      </c>
-      <c r="C19" t="s">
-        <v>43</v>
-      </c>
-      <c r="D19" s="13" t="s">
-        <v>42</v>
       </c>
       <c r="E19" s="20"/>
       <c r="F19" s="20"/>
@@ -1171,19 +1172,19 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B20" t="s">
+        <v>44</v>
+      </c>
+      <c r="C20" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="E20" s="19" t="s">
-        <v>58</v>
       </c>
       <c r="F20" s="19"/>
       <c r="G20" s="19"/>
@@ -1194,19 +1195,19 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E21" s="19" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F21" s="19"/>
       <c r="G21" s="19"/>
@@ -1217,19 +1218,19 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
         <v>47</v>
       </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
       <c r="D22" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E22" s="19" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F22" s="19"/>
       <c r="G22" s="19"/>
@@ -1241,13 +1242,13 @@
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
         <v>49</v>
       </c>
-      <c r="C23" t="s">
-        <v>50</v>
-      </c>
       <c r="D23" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
@@ -1259,19 +1260,19 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B24" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" t="s">
         <v>51</v>
       </c>
-      <c r="C24" t="s">
-        <v>52</v>
-      </c>
       <c r="D24" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E24" s="19" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F24" s="19"/>
       <c r="G24" s="19"/>
@@ -1283,13 +1284,13 @@
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
@@ -1302,13 +1303,13 @@
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
+        <v>53</v>
+      </c>
+      <c r="C26" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="s">
-        <v>55</v>
-      </c>
       <c r="D26" s="13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>

</xml_diff>

<commit_message>
atividade 4 - modelagem parametrica
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -688,8 +688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -906,12 +906,16 @@
       <c r="G7" s="1">
         <v>10</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
+      <c r="H7" s="1">
+        <v>10</v>
+      </c>
+      <c r="I7" s="1">
+        <v>10</v>
+      </c>
       <c r="J7" s="1"/>
       <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="17">
@@ -1126,7 +1130,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>24.666666666666668</v>
+        <v>26.333333333333332</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
realização prova final disciplina Modelagem Paramétrica
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -220,7 +220,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,6 +247,13 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -328,7 +335,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -382,6 +389,26 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -689,7 +716,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="E20" sqref="E20:K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -912,10 +939,12 @@
       <c r="I7" s="1">
         <v>10</v>
       </c>
-      <c r="J7" s="1"/>
+      <c r="J7" s="1">
+        <v>48</v>
+      </c>
       <c r="K7" s="1">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="L7" s="1"/>
       <c r="M7" s="17">
@@ -926,13 +955,13 @@
       <c r="A8" s="9">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="23" t="s">
         <v>65</v>
       </c>
       <c r="E8" s="5"/>
@@ -952,13 +981,13 @@
       <c r="A9" s="8">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="26">
         <v>44177</v>
       </c>
       <c r="F9" s="1"/>
@@ -977,13 +1006,13 @@
       <c r="A10" s="9">
         <v>8</v>
       </c>
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="27">
         <v>43872</v>
       </c>
-      <c r="D10" s="7">
+      <c r="D10" s="27">
         <v>44177</v>
       </c>
       <c r="E10" s="5"/>
@@ -1003,13 +1032,13 @@
       <c r="A11" s="8">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="26">
         <v>44410</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" s="28" t="s">
         <v>27</v>
       </c>
       <c r="F11" s="1"/>
@@ -1028,13 +1057,13 @@
       <c r="A12" s="9">
         <v>10</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="D12" s="23" t="s">
         <v>27</v>
       </c>
       <c r="E12" s="5"/>
@@ -1054,13 +1083,13 @@
       <c r="A13" s="8">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="28" t="s">
         <v>28</v>
       </c>
       <c r="F13" s="1"/>
@@ -1079,13 +1108,13 @@
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="C14" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="D14" s="23" t="s">
         <v>28</v>
       </c>
       <c r="E14" s="5"/>
@@ -1105,13 +1134,13 @@
       <c r="A15" s="8">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" s="28" t="s">
         <v>29</v>
       </c>
       <c r="F15" s="1"/>
@@ -1130,7 +1159,7 @@
       </c>
       <c r="K16" s="12">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>26.333333333333332</v>
+        <v>30.333333333333332</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
teste unidade 1 - modelos informacionais
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -417,50 +417,50 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -768,7 +768,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M17" sqref="M17"/>
+      <selection activeCell="E18" sqref="E18:K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -873,14 +873,22 @@
         <v>62</v>
       </c>
       <c r="E4" s="5"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
+      <c r="F4" s="4">
+        <v>10</v>
+      </c>
+      <c r="G4" s="4">
+        <v>10</v>
+      </c>
+      <c r="H4" s="4">
+        <v>10</v>
+      </c>
+      <c r="I4" s="4">
+        <v>10</v>
+      </c>
       <c r="J4" s="4"/>
-      <c r="K4" s="36">
+      <c r="K4" s="34">
         <f t="shared" ref="K4:K15" si="0">F4+G4+H4+I4+J4</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L4" s="4"/>
       <c r="M4" s="17">
@@ -955,7 +963,7 @@
       <c r="J6" s="4">
         <v>54</v>
       </c>
-      <c r="K6" s="36">
+      <c r="K6" s="34">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
@@ -1006,16 +1014,16 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="29">
+      <c r="A8" s="27">
         <v>6</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="31" t="s">
+      <c r="C8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="29" t="s">
+      <c r="D8" s="27" t="s">
         <v>62</v>
       </c>
       <c r="E8" s="5"/>
@@ -1032,7 +1040,7 @@
         <v>10</v>
       </c>
       <c r="J8" s="4"/>
-      <c r="K8" s="36">
+      <c r="K8" s="34">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
@@ -1042,16 +1050,16 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="32">
+      <c r="A9" s="30">
         <v>7</v>
       </c>
-      <c r="B9" s="33" t="s">
+      <c r="B9" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="C9" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="35">
+      <c r="D9" s="33">
         <v>44177</v>
       </c>
       <c r="F9" s="1"/>
@@ -1087,7 +1095,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="36">
+      <c r="K10" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1138,7 +1146,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="36">
+      <c r="K12" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1189,7 +1197,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="36">
+      <c r="K14" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1197,38 +1205,38 @@
       <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="38">
+      <c r="A15" s="36">
         <v>13</v>
       </c>
-      <c r="B15" s="39" t="s">
+      <c r="B15" s="37" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="40" t="s">
+      <c r="C15" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="42"/>
-      <c r="F15" s="43"/>
-      <c r="G15" s="43"/>
-      <c r="H15" s="43"/>
-      <c r="I15" s="43"/>
-      <c r="J15" s="43"/>
-      <c r="K15" s="44">
+      <c r="E15" s="40"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="42">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="42"/>
-      <c r="M15" s="42"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="40"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="J16" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="K16" s="37">
+      <c r="K16" s="35">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>33.666666666666664</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1245,13 +1253,13 @@
       <c r="D18" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-      <c r="G18" s="28"/>
-      <c r="H18" s="28"/>
-      <c r="I18" s="28"/>
-      <c r="J18" s="28"/>
-      <c r="K18" s="28"/>
+      <c r="E18" s="44"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="44"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1264,13 +1272,13 @@
       <c r="D19" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-      <c r="G19" s="28"/>
-      <c r="H19" s="28"/>
-      <c r="I19" s="28"/>
-      <c r="J19" s="28"/>
-      <c r="K19" s="28"/>
+      <c r="E19" s="44"/>
+      <c r="F19" s="44"/>
+      <c r="G19" s="44"/>
+      <c r="H19" s="44"/>
+      <c r="I19" s="44"/>
+      <c r="J19" s="44"/>
+      <c r="K19" s="44"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1285,15 +1293,15 @@
       <c r="D20" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E20" s="27" t="s">
+      <c r="E20" s="43" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="27"/>
-      <c r="K20" s="27"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
+      <c r="K20" s="43"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1308,15 +1316,15 @@
       <c r="D21" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E21" s="27" t="s">
+      <c r="E21" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="F21" s="27"/>
-      <c r="G21" s="27"/>
-      <c r="H21" s="27"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="27"/>
-      <c r="K21" s="27"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+      <c r="K21" s="43"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1331,15 +1339,15 @@
       <c r="D22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E22" s="27" t="s">
+      <c r="E22" s="43" t="s">
         <v>56</v>
       </c>
-      <c r="F22" s="27"/>
-      <c r="G22" s="27"/>
-      <c r="H22" s="27"/>
-      <c r="I22" s="27"/>
-      <c r="J22" s="27"/>
-      <c r="K22" s="27"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -1352,13 +1360,13 @@
       <c r="D23" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="27"/>
-      <c r="K23" s="27"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+      <c r="K23" s="43"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1373,15 +1381,15 @@
       <c r="D24" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E24" s="27" t="s">
+      <c r="E24" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="F24" s="27"/>
-      <c r="G24" s="27"/>
-      <c r="H24" s="27"/>
-      <c r="I24" s="27"/>
-      <c r="J24" s="27"/>
-      <c r="K24" s="27"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+      <c r="K24" s="43"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1394,13 +1402,13 @@
       <c r="D25" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E25" s="27"/>
-      <c r="F25" s="27"/>
-      <c r="G25" s="27"/>
-      <c r="H25" s="27"/>
-      <c r="I25" s="27"/>
-      <c r="J25" s="27"/>
-      <c r="K25" s="27"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+      <c r="K25" s="43"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1413,13 +1421,13 @@
       <c r="D26" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
-      <c r="G26" s="27"/>
-      <c r="H26" s="27"/>
-      <c r="I26" s="27"/>
-      <c r="J26" s="27"/>
-      <c r="K26" s="27"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="43"/>
+      <c r="I26" s="43"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>

</xml_diff>

<commit_message>
prova modelos informãcionais e BIM 4D
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
   <si>
     <t>Disciplina</t>
   </si>
@@ -347,7 +347,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -461,6 +461,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -768,7 +774,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18:K18"/>
+      <selection activeCell="E21" sqref="E21:K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,12 +891,16 @@
       <c r="I4" s="4">
         <v>10</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="4">
+        <v>60</v>
+      </c>
       <c r="K4" s="34">
         <f t="shared" ref="K4:K15" si="0">F4+G4+H4+I4+J4</f>
-        <v>40</v>
-      </c>
-      <c r="L4" s="4"/>
+        <v>100</v>
+      </c>
+      <c r="L4" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="M4" s="17">
         <v>2</v>
       </c>
@@ -1039,12 +1049,16 @@
       <c r="I8" s="4">
         <v>10</v>
       </c>
-      <c r="J8" s="4"/>
+      <c r="J8" s="4">
+        <v>54</v>
+      </c>
       <c r="K8" s="34">
         <f t="shared" si="0"/>
-        <v>40</v>
-      </c>
-      <c r="L8" s="4"/>
+        <v>94</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>60</v>
+      </c>
       <c r="M8" s="17">
         <v>6</v>
       </c>
@@ -1095,7 +1109,7 @@
       <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
-      <c r="K10" s="34">
+      <c r="K10" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1120,7 +1134,7 @@
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
-      <c r="K11" s="14">
+      <c r="K11" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1146,7 +1160,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="34">
+      <c r="K12" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1171,7 +1185,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="14">
+      <c r="K13" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1197,7 +1211,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="34">
+      <c r="K14" s="45">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1236,7 +1250,7 @@
       </c>
       <c r="K16" s="35">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>37</v>
+        <v>46.5</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
abertura turma bim 7D
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -416,9 +416,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -465,22 +462,25 @@
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -787,8 +787,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:K26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -909,7 +909,7 @@
       <c r="J4" s="4">
         <v>60</v>
       </c>
-      <c r="K4" s="33">
+      <c r="K4" s="32">
         <f t="shared" ref="K4:K15" si="0">F4+G4+H4+I4+J4</f>
         <v>100</v>
       </c>
@@ -988,7 +988,7 @@
       <c r="J6" s="4">
         <v>54</v>
       </c>
-      <c r="K6" s="33">
+      <c r="K6" s="32">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
@@ -1039,16 +1039,16 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="26">
+      <c r="A8" s="25">
         <v>6</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="26" t="s">
+      <c r="D8" s="25" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="5"/>
@@ -1067,7 +1067,7 @@
       <c r="J8" s="4">
         <v>54</v>
       </c>
-      <c r="K8" s="33">
+      <c r="K8" s="32">
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
@@ -1079,16 +1079,16 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="29">
+      <c r="A9" s="28">
         <v>7</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="32">
+      <c r="D9" s="31">
         <v>44177</v>
       </c>
       <c r="F9" s="1">
@@ -1116,62 +1116,63 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="26">
+      <c r="A10" s="25">
         <v>8</v>
       </c>
-      <c r="B10" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="45">
+      <c r="B10" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="42">
         <v>43872</v>
       </c>
-      <c r="D10" s="45">
+      <c r="D10" s="42">
         <v>44177</v>
       </c>
-      <c r="E10" s="27"/>
-      <c r="F10" s="26">
-        <v>10</v>
-      </c>
-      <c r="G10" s="26">
+      <c r="E10" s="26"/>
+      <c r="F10" s="25">
+        <v>10</v>
+      </c>
+      <c r="G10" s="25">
         <v>8.75</v>
       </c>
-      <c r="H10" s="26">
-        <v>10</v>
-      </c>
-      <c r="I10" s="26">
-        <v>10</v>
-      </c>
-      <c r="J10" s="26"/>
-      <c r="K10" s="46">
+      <c r="H10" s="25">
+        <v>10</v>
+      </c>
+      <c r="I10" s="25">
+        <v>10</v>
+      </c>
+      <c r="J10" s="25"/>
+      <c r="K10" s="43">
         <f t="shared" si="0"/>
         <v>38.75</v>
       </c>
-      <c r="L10" s="26"/>
+      <c r="L10" s="25"/>
       <c r="M10" s="16"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="28">
         <v>9</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="24">
+      <c r="C11" s="31">
         <v>44410</v>
       </c>
-      <c r="D11" s="25" t="s">
+      <c r="D11" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="42">
+      <c r="E11" s="29"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="48">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L11" s="1"/>
+      <c r="L11" s="28"/>
       <c r="M11" s="16"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -1193,7 +1194,7 @@
       <c r="H12" s="4"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
-      <c r="K12" s="41">
+      <c r="K12" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1210,7 +1211,7 @@
       <c r="C13" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="24" t="s">
         <v>25</v>
       </c>
       <c r="F13" s="1"/>
@@ -1218,7 +1219,7 @@
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
-      <c r="K13" s="42">
+      <c r="K13" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1244,7 +1245,7 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="41">
+      <c r="K14" s="40">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -1252,36 +1253,36 @@
       <c r="M14" s="18"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="34">
+      <c r="A15" s="33">
         <v>13</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="34" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="36" t="s">
+      <c r="C15" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="37" t="s">
+      <c r="D15" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
-      <c r="G15" s="39"/>
-      <c r="H15" s="39"/>
-      <c r="I15" s="39"/>
-      <c r="J15" s="39"/>
-      <c r="K15" s="40">
+      <c r="E15" s="37"/>
+      <c r="F15" s="38"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="38"/>
+      <c r="J15" s="38"/>
+      <c r="K15" s="39">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="38"/>
-      <c r="M15" s="38"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="37"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J16" s="48" t="s">
+      <c r="J16" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="47">
+      <c r="K16" s="44">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
         <v>55.729166666666664</v>
       </c>
@@ -1300,13 +1301,13 @@
       <c r="D18" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="44"/>
-      <c r="F18" s="44"/>
-      <c r="G18" s="44"/>
-      <c r="H18" s="44"/>
-      <c r="I18" s="44"/>
-      <c r="J18" s="44"/>
-      <c r="K18" s="44"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="47"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
+      <c r="K18" s="47"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1319,13 +1320,13 @@
       <c r="D19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="44"/>
-      <c r="F19" s="44"/>
-      <c r="G19" s="44"/>
-      <c r="H19" s="44"/>
-      <c r="I19" s="44"/>
-      <c r="J19" s="44"/>
-      <c r="K19" s="44"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="47"/>
+      <c r="G19" s="47"/>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="47"/>
+      <c r="K19" s="47"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1340,15 +1341,15 @@
       <c r="D20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="43"/>
-      <c r="G20" s="43"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="43"/>
-      <c r="J20" s="43"/>
-      <c r="K20" s="43"/>
+      <c r="F20" s="46"/>
+      <c r="G20" s="46"/>
+      <c r="H20" s="46"/>
+      <c r="I20" s="46"/>
+      <c r="J20" s="46"/>
+      <c r="K20" s="46"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1363,15 +1364,15 @@
       <c r="D21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="43"/>
-      <c r="G21" s="43"/>
-      <c r="H21" s="43"/>
-      <c r="I21" s="43"/>
-      <c r="J21" s="43"/>
-      <c r="K21" s="43"/>
+      <c r="F21" s="46"/>
+      <c r="G21" s="46"/>
+      <c r="H21" s="46"/>
+      <c r="I21" s="46"/>
+      <c r="J21" s="46"/>
+      <c r="K21" s="46"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1386,15 +1387,15 @@
       <c r="D22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="43" t="s">
+      <c r="E22" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
-      <c r="I22" s="43"/>
-      <c r="J22" s="43"/>
-      <c r="K22" s="43"/>
+      <c r="F22" s="46"/>
+      <c r="G22" s="46"/>
+      <c r="H22" s="46"/>
+      <c r="I22" s="46"/>
+      <c r="J22" s="46"/>
+      <c r="K22" s="46"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -1407,13 +1408,13 @@
       <c r="D23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="43"/>
-      <c r="F23" s="43"/>
-      <c r="G23" s="43"/>
-      <c r="H23" s="43"/>
-      <c r="I23" s="43"/>
-      <c r="J23" s="43"/>
-      <c r="K23" s="43"/>
+      <c r="E23" s="46"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
+      <c r="I23" s="46"/>
+      <c r="J23" s="46"/>
+      <c r="K23" s="46"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1428,15 +1429,15 @@
       <c r="D24" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="43"/>
-      <c r="G24" s="43"/>
-      <c r="H24" s="43"/>
-      <c r="I24" s="43"/>
-      <c r="J24" s="43"/>
-      <c r="K24" s="43"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1449,13 +1450,13 @@
       <c r="D25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="43"/>
-      <c r="G25" s="43"/>
-      <c r="H25" s="43"/>
-      <c r="I25" s="43"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
+      <c r="E25" s="46"/>
+      <c r="F25" s="46"/>
+      <c r="G25" s="46"/>
+      <c r="H25" s="46"/>
+      <c r="I25" s="46"/>
+      <c r="J25" s="46"/>
+      <c r="K25" s="46"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1468,13 +1469,13 @@
       <c r="D26" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="43"/>
-      <c r="F26" s="43"/>
-      <c r="G26" s="43"/>
-      <c r="H26" s="43"/>
-      <c r="I26" s="43"/>
-      <c r="J26" s="43"/>
-      <c r="K26" s="43"/>
+      <c r="E26" s="46"/>
+      <c r="F26" s="46"/>
+      <c r="G26" s="46"/>
+      <c r="H26" s="46"/>
+      <c r="I26" s="46"/>
+      <c r="J26" s="46"/>
+      <c r="K26" s="46"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>

</xml_diff>

<commit_message>
puc espec. BIM - prova módulo energético
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t>Disciplina</t>
   </si>
@@ -474,13 +474,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -788,14 +788,15 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="4.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -1110,7 +1111,9 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="L9" s="1"/>
+      <c r="L9" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="M9" s="17">
         <v>7</v>
       </c>
@@ -1141,13 +1144,19 @@
       <c r="I10" s="25">
         <v>10</v>
       </c>
-      <c r="J10" s="25"/>
+      <c r="J10" s="25">
+        <v>48</v>
+      </c>
       <c r="K10" s="43">
         <f t="shared" si="0"/>
-        <v>38.75</v>
-      </c>
-      <c r="L10" s="25"/>
-      <c r="M10" s="16"/>
+        <v>86.75</v>
+      </c>
+      <c r="L10" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="M10" s="17">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="28">
@@ -1168,12 +1177,14 @@
       <c r="H11" s="28"/>
       <c r="I11" s="28"/>
       <c r="J11" s="28"/>
-      <c r="K11" s="48">
+      <c r="K11" s="46">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L11" s="28"/>
-      <c r="M11" s="16"/>
+      <c r="M11" s="17">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
@@ -1284,7 +1295,7 @@
       </c>
       <c r="K16" s="44">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>55.729166666666664</v>
+        <v>59.729166666666664</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1301,13 +1312,13 @@
       <c r="D18" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="47"/>
-      <c r="F18" s="47"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
-      <c r="K18" s="47"/>
+      <c r="E18" s="48"/>
+      <c r="F18" s="48"/>
+      <c r="G18" s="48"/>
+      <c r="H18" s="48"/>
+      <c r="I18" s="48"/>
+      <c r="J18" s="48"/>
+      <c r="K18" s="48"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1320,13 +1331,13 @@
       <c r="D19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="47"/>
-      <c r="F19" s="47"/>
-      <c r="G19" s="47"/>
-      <c r="H19" s="47"/>
-      <c r="I19" s="47"/>
-      <c r="J19" s="47"/>
-      <c r="K19" s="47"/>
+      <c r="E19" s="48"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="48"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
+      <c r="K19" s="48"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1341,15 +1352,15 @@
       <c r="D20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="46" t="s">
+      <c r="E20" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="46"/>
-      <c r="G20" s="46"/>
-      <c r="H20" s="46"/>
-      <c r="I20" s="46"/>
-      <c r="J20" s="46"/>
-      <c r="K20" s="46"/>
+      <c r="F20" s="47"/>
+      <c r="G20" s="47"/>
+      <c r="H20" s="47"/>
+      <c r="I20" s="47"/>
+      <c r="J20" s="47"/>
+      <c r="K20" s="47"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1364,15 +1375,15 @@
       <c r="D21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="46" t="s">
+      <c r="E21" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="46"/>
-      <c r="G21" s="46"/>
-      <c r="H21" s="46"/>
-      <c r="I21" s="46"/>
-      <c r="J21" s="46"/>
-      <c r="K21" s="46"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1387,15 +1398,15 @@
       <c r="D22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="46" t="s">
+      <c r="E22" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="46"/>
-      <c r="G22" s="46"/>
-      <c r="H22" s="46"/>
-      <c r="I22" s="46"/>
-      <c r="J22" s="46"/>
-      <c r="K22" s="46"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -1408,13 +1419,13 @@
       <c r="D23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="46"/>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
-      <c r="I23" s="46"/>
-      <c r="J23" s="46"/>
-      <c r="K23" s="46"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="47"/>
+      <c r="G23" s="47"/>
+      <c r="H23" s="47"/>
+      <c r="I23" s="47"/>
+      <c r="J23" s="47"/>
+      <c r="K23" s="47"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1429,15 +1440,15 @@
       <c r="D24" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="46" t="s">
+      <c r="E24" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="46"/>
-      <c r="G24" s="46"/>
-      <c r="H24" s="46"/>
-      <c r="I24" s="46"/>
-      <c r="J24" s="46"/>
-      <c r="K24" s="46"/>
+      <c r="F24" s="47"/>
+      <c r="G24" s="47"/>
+      <c r="H24" s="47"/>
+      <c r="I24" s="47"/>
+      <c r="J24" s="47"/>
+      <c r="K24" s="47"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1450,13 +1461,13 @@
       <c r="D25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="46"/>
-      <c r="F25" s="46"/>
-      <c r="G25" s="46"/>
-      <c r="H25" s="46"/>
-      <c r="I25" s="46"/>
-      <c r="J25" s="46"/>
-      <c r="K25" s="46"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="47"/>
+      <c r="G25" s="47"/>
+      <c r="H25" s="47"/>
+      <c r="I25" s="47"/>
+      <c r="J25" s="47"/>
+      <c r="K25" s="47"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1469,13 +1480,13 @@
       <c r="D26" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="47"/>
+      <c r="G26" s="47"/>
+      <c r="H26" s="47"/>
+      <c r="I26" s="47"/>
+      <c r="J26" s="47"/>
+      <c r="K26" s="47"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>

</xml_diff>

<commit_message>
provas gestão de instalações e segurança
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
   <si>
     <t>Disciplina</t>
   </si>
@@ -355,7 +355,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -396,9 +396,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -412,13 +409,6 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,9 +449,6 @@
     <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -481,6 +468,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -788,7 +778,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="M20" sqref="M20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,14 +900,14 @@
       <c r="J4" s="4">
         <v>60</v>
       </c>
-      <c r="K4" s="32">
+      <c r="K4" s="28">
         <f t="shared" ref="K4:K15" si="0">F4+G4+H4+I4+J4</f>
         <v>100</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M4" s="17">
+      <c r="M4" s="16">
         <v>2</v>
       </c>
     </row>
@@ -956,7 +946,7 @@
       <c r="L5" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M5" s="17">
+      <c r="M5" s="16">
         <v>3</v>
       </c>
     </row>
@@ -989,14 +979,14 @@
       <c r="J6" s="4">
         <v>54</v>
       </c>
-      <c r="K6" s="32">
+      <c r="K6" s="28">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
       <c r="L6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M6" s="17">
+      <c r="M6" s="16">
         <v>4</v>
       </c>
     </row>
@@ -1035,21 +1025,21 @@
       <c r="L7" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M7" s="17">
+      <c r="M7" s="16">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="25">
+      <c r="A8" s="21">
         <v>6</v>
       </c>
-      <c r="B8" s="26" t="s">
+      <c r="B8" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="21" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="5"/>
@@ -1068,28 +1058,28 @@
       <c r="J8" s="4">
         <v>54</v>
       </c>
-      <c r="K8" s="32">
+      <c r="K8" s="28">
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
       <c r="L8" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="M8" s="17">
+      <c r="M8" s="16">
         <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="28">
+      <c r="A9" s="24">
         <v>7</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="27">
         <v>44177</v>
       </c>
       <c r="F9" s="1">
@@ -1114,140 +1104,166 @@
       <c r="L9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="M9" s="17">
+      <c r="M9" s="16">
         <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="25">
+      <c r="A10" s="21">
         <v>8</v>
       </c>
-      <c r="B10" s="26" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="42">
+      <c r="B10" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="37">
         <v>43872</v>
       </c>
-      <c r="D10" s="42">
+      <c r="D10" s="37">
         <v>44177</v>
       </c>
-      <c r="E10" s="26"/>
-      <c r="F10" s="25">
-        <v>10</v>
-      </c>
-      <c r="G10" s="25">
+      <c r="E10" s="22"/>
+      <c r="F10" s="21">
+        <v>10</v>
+      </c>
+      <c r="G10" s="21">
         <v>8.75</v>
       </c>
-      <c r="H10" s="25">
-        <v>10</v>
-      </c>
-      <c r="I10" s="25">
-        <v>10</v>
-      </c>
-      <c r="J10" s="25">
+      <c r="H10" s="21">
+        <v>10</v>
+      </c>
+      <c r="I10" s="21">
+        <v>10</v>
+      </c>
+      <c r="J10" s="21">
         <v>48</v>
       </c>
-      <c r="K10" s="43">
+      <c r="K10" s="38">
         <f t="shared" si="0"/>
         <v>86.75</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="M10" s="17">
+      <c r="M10" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="28">
+      <c r="A11" s="24">
         <v>9</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="31">
+      <c r="C11" s="27">
         <v>44410</v>
       </c>
-      <c r="D11" s="28" t="s">
+      <c r="D11" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="29"/>
-      <c r="F11" s="28"/>
-      <c r="G11" s="28"/>
-      <c r="H11" s="28"/>
-      <c r="I11" s="28"/>
-      <c r="J11" s="28"/>
-      <c r="K11" s="46">
+      <c r="E11" s="25"/>
+      <c r="F11" s="24">
+        <v>10</v>
+      </c>
+      <c r="G11" s="24">
+        <v>10</v>
+      </c>
+      <c r="H11" s="24">
+        <v>10</v>
+      </c>
+      <c r="I11" s="24">
+        <v>10</v>
+      </c>
+      <c r="J11" s="24">
+        <v>48</v>
+      </c>
+      <c r="K11" s="41">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L11" s="28"/>
-      <c r="M11" s="17">
+        <v>88</v>
+      </c>
+      <c r="L11" s="24"/>
+      <c r="M11" s="16">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>10</v>
-      </c>
-      <c r="B12" s="19" t="s">
+      <c r="A12" s="21">
+        <v>10</v>
+      </c>
+      <c r="B12" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="23" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="21" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="5"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="4"/>
-      <c r="J12" s="4"/>
-      <c r="K12" s="40">
+      <c r="F12" s="4">
+        <v>10</v>
+      </c>
+      <c r="G12" s="4">
+        <v>10</v>
+      </c>
+      <c r="H12" s="4">
+        <v>10</v>
+      </c>
+      <c r="I12" s="4">
+        <v>10</v>
+      </c>
+      <c r="J12" s="4">
+        <v>42</v>
+      </c>
+      <c r="K12" s="38">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L12" s="4"/>
-      <c r="M12" s="16"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+        <v>82</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="M12" s="16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="24">
         <v>11</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="26" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="24" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
+      <c r="I13" s="24"/>
+      <c r="J13" s="24"/>
       <c r="K13" s="41">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="1"/>
-      <c r="M13" s="16"/>
+      <c r="L13" s="24"/>
+      <c r="M13" s="44">
+        <v>11</v>
+      </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>12</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="20" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="5"/>
@@ -1256,46 +1272,46 @@
       <c r="H14" s="4"/>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
-      <c r="K14" s="40">
+      <c r="K14" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="L14" s="4"/>
-      <c r="M14" s="18"/>
+      <c r="M14" s="17"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="33">
+      <c r="A15" s="29">
         <v>13</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="35" t="s">
+      <c r="C15" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="36" t="s">
+      <c r="D15" s="32" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="37"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
-      <c r="K15" s="39">
+      <c r="E15" s="33"/>
+      <c r="F15" s="34"/>
+      <c r="G15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="34"/>
+      <c r="J15" s="34"/>
+      <c r="K15" s="35">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="37"/>
-      <c r="M15" s="37"/>
+      <c r="L15" s="33"/>
+      <c r="M15" s="33"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J16" s="45" t="s">
+      <c r="J16" s="40" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="44">
+      <c r="K16" s="39">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>59.729166666666664</v>
+        <v>73.895833333333329</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1312,13 +1328,13 @@
       <c r="D18" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="48"/>
-      <c r="J18" s="48"/>
-      <c r="K18" s="48"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
+      <c r="K18" s="43"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1331,13 +1347,13 @@
       <c r="D19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="48"/>
-      <c r="F19" s="48"/>
-      <c r="G19" s="48"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
-      <c r="K19" s="48"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1352,15 +1368,15 @@
       <c r="D20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="47" t="s">
+      <c r="E20" s="42" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="47"/>
-      <c r="G20" s="47"/>
-      <c r="H20" s="47"/>
-      <c r="I20" s="47"/>
-      <c r="J20" s="47"/>
-      <c r="K20" s="47"/>
+      <c r="F20" s="42"/>
+      <c r="G20" s="42"/>
+      <c r="H20" s="42"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="42"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1375,15 +1391,15 @@
       <c r="D21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="47" t="s">
+      <c r="E21" s="42" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="47"/>
-      <c r="G21" s="47"/>
-      <c r="H21" s="47"/>
-      <c r="I21" s="47"/>
-      <c r="J21" s="47"/>
-      <c r="K21" s="47"/>
+      <c r="F21" s="42"/>
+      <c r="G21" s="42"/>
+      <c r="H21" s="42"/>
+      <c r="I21" s="42"/>
+      <c r="J21" s="42"/>
+      <c r="K21" s="42"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1398,15 +1414,15 @@
       <c r="D22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="47" t="s">
+      <c r="E22" s="42" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="47"/>
-      <c r="G22" s="47"/>
-      <c r="H22" s="47"/>
-      <c r="I22" s="47"/>
-      <c r="J22" s="47"/>
-      <c r="K22" s="47"/>
+      <c r="F22" s="42"/>
+      <c r="G22" s="42"/>
+      <c r="H22" s="42"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="42"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -1419,13 +1435,13 @@
       <c r="D23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="47"/>
-      <c r="F23" s="47"/>
-      <c r="G23" s="47"/>
-      <c r="H23" s="47"/>
-      <c r="I23" s="47"/>
-      <c r="J23" s="47"/>
-      <c r="K23" s="47"/>
+      <c r="E23" s="42"/>
+      <c r="F23" s="42"/>
+      <c r="G23" s="42"/>
+      <c r="H23" s="42"/>
+      <c r="I23" s="42"/>
+      <c r="J23" s="42"/>
+      <c r="K23" s="42"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1440,15 +1456,15 @@
       <c r="D24" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="47" t="s">
+      <c r="E24" s="42" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="47"/>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="47"/>
-      <c r="J24" s="47"/>
-      <c r="K24" s="47"/>
+      <c r="F24" s="42"/>
+      <c r="G24" s="42"/>
+      <c r="H24" s="42"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="42"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1461,13 +1477,13 @@
       <c r="D25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="47"/>
-      <c r="F25" s="47"/>
-      <c r="G25" s="47"/>
-      <c r="H25" s="47"/>
-      <c r="I25" s="47"/>
-      <c r="J25" s="47"/>
-      <c r="K25" s="47"/>
+      <c r="E25" s="42"/>
+      <c r="F25" s="42"/>
+      <c r="G25" s="42"/>
+      <c r="H25" s="42"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="42"/>
+      <c r="K25" s="42"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1480,13 +1496,13 @@
       <c r="D26" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="47"/>
-      <c r="F26" s="47"/>
-      <c r="G26" s="47"/>
-      <c r="H26" s="47"/>
-      <c r="I26" s="47"/>
-      <c r="J26" s="47"/>
-      <c r="K26" s="47"/>
+      <c r="E26" s="42"/>
+      <c r="F26" s="42"/>
+      <c r="G26" s="42"/>
+      <c r="H26" s="42"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="42"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>

</xml_diff>

<commit_message>
teste unidade 4 10D
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -305,7 +305,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -337,25 +337,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -399,16 +386,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -446,9 +423,6 @@
     <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -462,15 +436,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -778,7 +752,7 @@
   <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,7 +874,7 @@
       <c r="J4" s="4">
         <v>60</v>
       </c>
-      <c r="K4" s="28">
+      <c r="K4" s="24">
         <f t="shared" ref="K4:K15" si="0">F4+G4+H4+I4+J4</f>
         <v>100</v>
       </c>
@@ -979,7 +953,7 @@
       <c r="J6" s="4">
         <v>54</v>
       </c>
-      <c r="K6" s="28">
+      <c r="K6" s="24">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
@@ -1030,16 +1004,16 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="21">
+      <c r="A8" s="17">
         <v>6</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="17" t="s">
         <v>61</v>
       </c>
       <c r="E8" s="5"/>
@@ -1058,7 +1032,7 @@
       <c r="J8" s="4">
         <v>54</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="24">
         <f t="shared" si="0"/>
         <v>94</v>
       </c>
@@ -1070,16 +1044,16 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="24">
+      <c r="A9" s="20">
         <v>7</v>
       </c>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="27">
+      <c r="D9" s="23">
         <v>44177</v>
       </c>
       <c r="F9" s="1">
@@ -1109,39 +1083,39 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="21">
+      <c r="A10" s="17">
         <v>8</v>
       </c>
-      <c r="B10" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" s="37">
+      <c r="B10" s="18" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="32">
         <v>43872</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="32">
         <v>44177</v>
       </c>
-      <c r="E10" s="22"/>
-      <c r="F10" s="21">
-        <v>10</v>
-      </c>
-      <c r="G10" s="21">
+      <c r="E10" s="18"/>
+      <c r="F10" s="17">
+        <v>10</v>
+      </c>
+      <c r="G10" s="17">
         <v>8.75</v>
       </c>
-      <c r="H10" s="21">
-        <v>10</v>
-      </c>
-      <c r="I10" s="21">
-        <v>10</v>
-      </c>
-      <c r="J10" s="21">
+      <c r="H10" s="17">
+        <v>10</v>
+      </c>
+      <c r="I10" s="17">
+        <v>10</v>
+      </c>
+      <c r="J10" s="17">
         <v>48</v>
       </c>
-      <c r="K10" s="38">
+      <c r="K10" s="33">
         <f t="shared" si="0"/>
         <v>86.75</v>
       </c>
-      <c r="L10" s="21" t="s">
+      <c r="L10" s="17" t="s">
         <v>59</v>
       </c>
       <c r="M10" s="16">
@@ -1149,54 +1123,54 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="24">
+      <c r="A11" s="20">
         <v>9</v>
       </c>
-      <c r="B11" s="25" t="s">
+      <c r="B11" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="C11" s="27">
+      <c r="C11" s="23">
         <v>44410</v>
       </c>
-      <c r="D11" s="24" t="s">
+      <c r="D11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="25"/>
-      <c r="F11" s="24">
-        <v>10</v>
-      </c>
-      <c r="G11" s="24">
-        <v>10</v>
-      </c>
-      <c r="H11" s="24">
-        <v>10</v>
-      </c>
-      <c r="I11" s="24">
-        <v>10</v>
-      </c>
-      <c r="J11" s="24">
+      <c r="E11" s="21"/>
+      <c r="F11" s="20">
+        <v>10</v>
+      </c>
+      <c r="G11" s="20">
+        <v>10</v>
+      </c>
+      <c r="H11" s="20">
+        <v>10</v>
+      </c>
+      <c r="I11" s="20">
+        <v>10</v>
+      </c>
+      <c r="J11" s="20">
         <v>48</v>
       </c>
-      <c r="K11" s="41">
+      <c r="K11" s="36">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="L11" s="24"/>
+      <c r="L11" s="20"/>
       <c r="M11" s="16">
         <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="21">
-        <v>10</v>
-      </c>
-      <c r="B12" s="22" t="s">
+      <c r="A12" s="17">
+        <v>10</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="17" t="s">
         <v>24</v>
       </c>
       <c r="E12" s="5"/>
@@ -1215,7 +1189,7 @@
       <c r="J12" s="4">
         <v>42</v>
       </c>
-      <c r="K12" s="38">
+      <c r="K12" s="33">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
@@ -1226,35 +1200,35 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:13" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24">
+    <row r="13" spans="1:13" s="21" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="20">
         <v>11</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="24"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="41">
+      <c r="F13" s="20"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20"/>
+      <c r="J13" s="20"/>
+      <c r="K13" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L13" s="24"/>
-      <c r="M13" s="44">
+      <c r="L13" s="20"/>
+      <c r="M13" s="37">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
+      <c r="A14" s="17">
         <v>12</v>
       </c>
       <c r="B14" s="18" t="s">
@@ -1263,55 +1237,65 @@
       <c r="C14" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="5"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="4"/>
-      <c r="J14" s="4"/>
-      <c r="K14" s="36">
+      <c r="E14" s="18"/>
+      <c r="F14" s="17">
+        <v>10</v>
+      </c>
+      <c r="G14" s="17">
+        <v>10</v>
+      </c>
+      <c r="H14" s="17">
+        <v>10</v>
+      </c>
+      <c r="I14" s="17">
+        <v>10</v>
+      </c>
+      <c r="J14" s="17"/>
+      <c r="K14" s="33">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="L14" s="17"/>
+      <c r="M14" s="37">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="25">
+        <v>13</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="30"/>
+      <c r="K15" s="31">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L14" s="4"/>
-      <c r="M14" s="17"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="29">
-        <v>13</v>
-      </c>
-      <c r="B15" s="30" t="s">
-        <v>7</v>
-      </c>
-      <c r="C15" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="D15" s="32" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="33"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-      <c r="I15" s="34"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L15" s="33"/>
-      <c r="M15" s="33"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="29"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J16" s="40" t="s">
+      <c r="J16" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="K16" s="39">
+      <c r="K16" s="34">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>73.895833333333329</v>
+        <v>77.229166666666671</v>
       </c>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
@@ -1328,13 +1312,13 @@
       <c r="D18" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E18" s="43"/>
-      <c r="F18" s="43"/>
-      <c r="G18" s="43"/>
-      <c r="H18" s="43"/>
-      <c r="I18" s="43"/>
-      <c r="J18" s="43"/>
-      <c r="K18" s="43"/>
+      <c r="E18" s="39"/>
+      <c r="F18" s="39"/>
+      <c r="G18" s="39"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="39"/>
+      <c r="J18" s="39"/>
+      <c r="K18" s="39"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
@@ -1347,13 +1331,13 @@
       <c r="D19" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E19" s="43"/>
-      <c r="F19" s="43"/>
-      <c r="G19" s="43"/>
-      <c r="H19" s="43"/>
-      <c r="I19" s="43"/>
-      <c r="J19" s="43"/>
-      <c r="K19" s="43"/>
+      <c r="E19" s="39"/>
+      <c r="F19" s="39"/>
+      <c r="G19" s="39"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="39"/>
+      <c r="J19" s="39"/>
+      <c r="K19" s="39"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
@@ -1368,15 +1352,15 @@
       <c r="D20" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E20" s="42" t="s">
+      <c r="E20" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="F20" s="42"/>
-      <c r="G20" s="42"/>
-      <c r="H20" s="42"/>
-      <c r="I20" s="42"/>
-      <c r="J20" s="42"/>
-      <c r="K20" s="42"/>
+      <c r="F20" s="38"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="38"/>
+      <c r="J20" s="38"/>
+      <c r="K20" s="38"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
@@ -1391,15 +1375,15 @@
       <c r="D21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E21" s="42" t="s">
+      <c r="E21" s="38" t="s">
         <v>56</v>
       </c>
-      <c r="F21" s="42"/>
-      <c r="G21" s="42"/>
-      <c r="H21" s="42"/>
-      <c r="I21" s="42"/>
-      <c r="J21" s="42"/>
-      <c r="K21" s="42"/>
+      <c r="F21" s="38"/>
+      <c r="G21" s="38"/>
+      <c r="H21" s="38"/>
+      <c r="I21" s="38"/>
+      <c r="J21" s="38"/>
+      <c r="K21" s="38"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
@@ -1414,15 +1398,15 @@
       <c r="D22" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E22" s="42" t="s">
+      <c r="E22" s="38" t="s">
         <v>55</v>
       </c>
-      <c r="F22" s="42"/>
-      <c r="G22" s="42"/>
-      <c r="H22" s="42"/>
-      <c r="I22" s="42"/>
-      <c r="J22" s="42"/>
-      <c r="K22" s="42"/>
+      <c r="F22" s="38"/>
+      <c r="G22" s="38"/>
+      <c r="H22" s="38"/>
+      <c r="I22" s="38"/>
+      <c r="J22" s="38"/>
+      <c r="K22" s="38"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
@@ -1435,13 +1419,13 @@
       <c r="D23" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
-      <c r="I23" s="42"/>
-      <c r="J23" s="42"/>
-      <c r="K23" s="42"/>
+      <c r="E23" s="38"/>
+      <c r="F23" s="38"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="38"/>
+      <c r="I23" s="38"/>
+      <c r="J23" s="38"/>
+      <c r="K23" s="38"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
@@ -1456,15 +1440,15 @@
       <c r="D24" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
+      <c r="K24" s="38"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
@@ -1477,13 +1461,13 @@
       <c r="D25" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
-      <c r="G25" s="42"/>
-      <c r="H25" s="42"/>
-      <c r="I25" s="42"/>
-      <c r="J25" s="42"/>
-      <c r="K25" s="42"/>
+      <c r="E25" s="38"/>
+      <c r="F25" s="38"/>
+      <c r="G25" s="38"/>
+      <c r="H25" s="38"/>
+      <c r="I25" s="38"/>
+      <c r="J25" s="38"/>
+      <c r="K25" s="38"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
@@ -1496,13 +1480,13 @@
       <c r="D26" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
-      <c r="G26" s="42"/>
-      <c r="H26" s="42"/>
-      <c r="I26" s="42"/>
-      <c r="J26" s="42"/>
-      <c r="K26" s="42"/>
+      <c r="E26" s="38"/>
+      <c r="F26" s="38"/>
+      <c r="G26" s="38"/>
+      <c r="H26" s="38"/>
+      <c r="I26" s="38"/>
+      <c r="J26" s="38"/>
+      <c r="K26" s="38"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>

</xml_diff>

<commit_message>
Reorganizando repo e inseriondo base dwg quinta monroy
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Plan1" sheetId="1" r:id="rId1"/>
-    <sheet name="Plan2" sheetId="2" r:id="rId2"/>
+    <sheet name="caldendário e notas" sheetId="1" r:id="rId1"/>
+    <sheet name="Ementas" sheetId="2" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="62">
   <si>
     <t>Disciplina</t>
   </si>
@@ -96,9 +96,6 @@
     <t>26/05/2021</t>
   </si>
   <si>
-    <t>31/10/2021</t>
-  </si>
-  <si>
     <t>Atividades</t>
   </si>
   <si>
@@ -177,18 +174,6 @@
     <t>**</t>
   </si>
   <si>
-    <t>Automação de verif. de projetos BIM</t>
-  </si>
-  <si>
-    <t>Membro do comite BIM</t>
-  </si>
-  <si>
-    <t>Professor e doutorando</t>
-  </si>
-  <si>
-    <t>Produção</t>
-  </si>
-  <si>
     <t xml:space="preserve">AP </t>
   </si>
   <si>
@@ -214,13 +199,16 @@
   </si>
   <si>
     <t>Média geral</t>
+  </si>
+  <si>
+    <t>15/08/2021</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -247,13 +235,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -342,7 +323,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -386,65 +367,52 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -749,10 +717,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M30"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -760,7 +728,7 @@
     <col min="2" max="2" width="40.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="4.85546875" customWidth="1"/>
+    <col min="5" max="5" width="3.7109375" customWidth="1"/>
     <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="10" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
@@ -769,7 +737,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -785,25 +753,25 @@
       </c>
       <c r="E2" s="12"/>
       <c r="F2" s="11" t="s">
+        <v>27</v>
+      </c>
+      <c r="G2" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="H2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="I2" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>33</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -839,7 +807,7 @@
         <v>86</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="M3" s="15">
         <v>1</v>
@@ -856,9 +824,8 @@
         <v>43898</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="E4" s="5"/>
+        <v>56</v>
+      </c>
       <c r="F4" s="4">
         <v>10</v>
       </c>
@@ -879,7 +846,7 @@
         <v>100</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M4" s="16">
         <v>2</v>
@@ -918,7 +885,7 @@
         <v>100</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M5" s="16">
         <v>3</v>
@@ -935,9 +902,8 @@
         <v>14</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="E6" s="5"/>
+        <v>53</v>
+      </c>
       <c r="F6" s="4">
         <v>8</v>
       </c>
@@ -958,7 +924,7 @@
         <v>90</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M6" s="16">
         <v>4</v>
@@ -975,7 +941,7 @@
         <v>43898</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="F7" s="1">
         <v>10</v>
@@ -997,7 +963,7 @@
         <v>88</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M7" s="16">
         <v>5</v>
@@ -1014,9 +980,8 @@
         <v>15</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>61</v>
-      </c>
-      <c r="E8" s="5"/>
+        <v>56</v>
+      </c>
       <c r="F8" s="4">
         <v>10</v>
       </c>
@@ -1037,7 +1002,7 @@
         <v>94</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M8" s="16">
         <v>6</v>
@@ -1076,7 +1041,7 @@
         <v>72</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M9" s="16">
         <v>7</v>
@@ -1089,13 +1054,12 @@
       <c r="B10" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="32">
+      <c r="C10" s="25">
         <v>43872</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="25">
         <v>44177</v>
       </c>
-      <c r="E10" s="18"/>
       <c r="F10" s="17">
         <v>10</v>
       </c>
@@ -1111,12 +1075,12 @@
       <c r="J10" s="17">
         <v>48</v>
       </c>
-      <c r="K10" s="33">
+      <c r="K10" s="26">
         <f t="shared" si="0"/>
         <v>86.75</v>
       </c>
       <c r="L10" s="17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M10" s="16">
         <v>8</v>
@@ -1127,7 +1091,7 @@
         <v>9</v>
       </c>
       <c r="B11" s="21" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C11" s="23">
         <v>44410</v>
@@ -1135,7 +1099,6 @@
       <c r="D11" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="21"/>
       <c r="F11" s="20">
         <v>10</v>
       </c>
@@ -1151,11 +1114,13 @@
       <c r="J11" s="20">
         <v>48</v>
       </c>
-      <c r="K11" s="36">
+      <c r="K11" s="29">
         <f t="shared" si="0"/>
         <v>88</v>
       </c>
-      <c r="L11" s="20"/>
+      <c r="L11" s="20" t="s">
+        <v>54</v>
+      </c>
       <c r="M11" s="16">
         <v>9</v>
       </c>
@@ -1165,7 +1130,7 @@
         <v>10</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C12" s="19" t="s">
         <v>17</v>
@@ -1173,7 +1138,6 @@
       <c r="D12" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="5"/>
       <c r="F12" s="4">
         <v>10</v>
       </c>
@@ -1189,12 +1153,12 @@
       <c r="J12" s="4">
         <v>42</v>
       </c>
-      <c r="K12" s="33">
+      <c r="K12" s="26">
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="M12" s="16">
         <v>10</v>
@@ -1205,7 +1169,7 @@
         <v>11</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="C13" s="22" t="s">
         <v>18</v>
@@ -1213,17 +1177,26 @@
       <c r="D13" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="20"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="20"/>
-      <c r="I13" s="20"/>
+      <c r="E13"/>
+      <c r="F13" s="20">
+        <v>10</v>
+      </c>
+      <c r="G13" s="20">
+        <v>10</v>
+      </c>
+      <c r="H13" s="20">
+        <v>10</v>
+      </c>
+      <c r="I13" s="20">
+        <v>10</v>
+      </c>
       <c r="J13" s="20"/>
-      <c r="K13" s="36">
+      <c r="K13" s="29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="L13" s="20"/>
-      <c r="M13" s="37">
+      <c r="M13" s="30">
         <v>11</v>
       </c>
     </row>
@@ -1240,7 +1213,6 @@
       <c r="D14" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="E14" s="18"/>
       <c r="F14" s="17">
         <v>10</v>
       </c>
@@ -1254,274 +1226,177 @@
         <v>10</v>
       </c>
       <c r="J14" s="17"/>
-      <c r="K14" s="33">
+      <c r="K14" s="26">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="L14" s="17"/>
-      <c r="M14" s="37">
+      <c r="M14" s="30">
         <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="25">
+      <c r="A15" s="31">
         <v>13</v>
       </c>
-      <c r="B15" s="26" t="s">
+      <c r="B15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="30"/>
-      <c r="I15" s="30"/>
-      <c r="J15" s="30"/>
-      <c r="K15" s="31">
+      <c r="D15" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="E15" s="32"/>
+      <c r="F15" s="31"/>
+      <c r="G15" s="31"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="31"/>
+      <c r="J15" s="31"/>
+      <c r="K15" s="34">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="L15" s="29"/>
-      <c r="M15" s="29"/>
+      <c r="L15" s="32"/>
+      <c r="M15" s="32"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="J16" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="K16" s="34">
+      <c r="J16" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="K16" s="27">
         <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>77.229166666666671</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="1"/>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+        <v>80.5625</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>35</v>
       </c>
       <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B19" t="s">
         <v>39</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E18" s="39"/>
-      <c r="F18" s="39"/>
-      <c r="G18" s="39"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="39"/>
-      <c r="J18" s="39"/>
-      <c r="K18" s="39"/>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="1"/>
-      <c r="B19" t="s">
-        <v>36</v>
       </c>
       <c r="C19" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="39"/>
-      <c r="F19" s="39"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="39"/>
-      <c r="J19" s="39"/>
-      <c r="K19" s="39"/>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B20" t="s">
         <v>40</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
-      <c r="K20" s="38"/>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D21" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="38" t="s">
-        <v>56</v>
-      </c>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
-      <c r="K21" s="38"/>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" t="s">
         <v>42</v>
       </c>
-      <c r="C22" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E22" s="38" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" s="38"/>
-      <c r="G22" s="38"/>
-      <c r="H22" s="38"/>
-      <c r="I22" s="38"/>
-      <c r="J22" s="38"/>
-      <c r="K22" s="38"/>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-      <c r="B23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" t="s">
-        <v>45</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E23" s="38"/>
-      <c r="F23" s="38"/>
-      <c r="G23" s="38"/>
-      <c r="H23" s="38"/>
-      <c r="I23" s="38"/>
-      <c r="J23" s="38"/>
-      <c r="K23" s="38"/>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="B24" t="s">
-        <v>46</v>
-      </c>
-      <c r="C24" t="s">
-        <v>47</v>
-      </c>
       <c r="D24" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E24" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
-      <c r="K24" s="38"/>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
         <v>48</v>
       </c>
       <c r="C25" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="38"/>
-      <c r="H25" s="38"/>
-      <c r="I25" s="38"/>
-      <c r="J25" s="38"/>
-      <c r="K25" s="38"/>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="1"/>
-      <c r="B26" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
-      <c r="D26" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="E26" s="38"/>
-      <c r="F26" s="38"/>
-      <c r="G26" s="38"/>
-      <c r="H26" s="38"/>
-      <c r="I26" s="38"/>
-      <c r="J26" s="38"/>
-      <c r="K26" s="38"/>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="1"/>
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="E26:K26"/>
-    <mergeCell ref="E25:K25"/>
-    <mergeCell ref="E23:K23"/>
-    <mergeCell ref="E18:K18"/>
-    <mergeCell ref="E19:K19"/>
-    <mergeCell ref="E20:K20"/>
-    <mergeCell ref="E21:K21"/>
-    <mergeCell ref="E22:K22"/>
-    <mergeCell ref="E24:K24"/>
-  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="D19" r:id="rId1"/>
-    <hyperlink ref="D18" r:id="rId2"/>
-    <hyperlink ref="D20" r:id="rId3"/>
-    <hyperlink ref="D21" r:id="rId4"/>
-    <hyperlink ref="D22" r:id="rId5"/>
-    <hyperlink ref="D23" r:id="rId6"/>
-    <hyperlink ref="D24" r:id="rId7"/>
-    <hyperlink ref="D25" r:id="rId8"/>
-    <hyperlink ref="D26" r:id="rId9"/>
+    <hyperlink ref="D18" r:id="rId1"/>
+    <hyperlink ref="D17" r:id="rId2"/>
+    <hyperlink ref="D19" r:id="rId3"/>
+    <hyperlink ref="D20" r:id="rId4"/>
+    <hyperlink ref="D21" r:id="rId5"/>
+    <hyperlink ref="D22" r:id="rId6"/>
+    <hyperlink ref="D23" r:id="rId7"/>
+    <hyperlink ref="D24" r:id="rId8"/>
+    <hyperlink ref="D25" r:id="rId9"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId10"/>
@@ -1544,7 +1419,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Realização provas BIM 9D e 10D
</commit_message>
<xml_diff>
--- a/cronograma_curso_provas.xlsx
+++ b/cronograma_curso_provas.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="caldendário e notas" sheetId="1" r:id="rId1"/>
-    <sheet name="Ementas" sheetId="2" r:id="rId2"/>
+    <sheet name="Ementas" sheetId="2" r:id="rId1"/>
+    <sheet name="caldendário e notas" sheetId="1" r:id="rId2"/>
     <sheet name="Plan3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -717,9 +717,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
@@ -1190,10 +1202,12 @@
       <c r="I13" s="20">
         <v>10</v>
       </c>
-      <c r="J13" s="20"/>
+      <c r="J13" s="20">
+        <v>48</v>
+      </c>
       <c r="K13" s="29">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="L13" s="20"/>
       <c r="M13" s="30">
@@ -1225,10 +1239,12 @@
       <c r="I14" s="17">
         <v>10</v>
       </c>
-      <c r="J14" s="17"/>
+      <c r="J14" s="17">
+        <v>48</v>
+      </c>
       <c r="K14" s="26">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>88</v>
       </c>
       <c r="L14" s="17"/>
       <c r="M14" s="30">
@@ -1266,8 +1282,8 @@
         <v>60</v>
       </c>
       <c r="K16" s="27">
-        <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14)/12</f>
-        <v>80.5625</v>
+        <f>(K3+K4+K5+K6+K7+K8+K9+K10+K11+K12+K13+K14+K15)/13</f>
+        <v>81.75</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1403,7 +1419,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
@@ -1413,16 +1429,4 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>